<commit_message>
addition of reference to Lancet Neurology article
</commit_message>
<xml_diff>
--- a/AED withdrawal relapse risk calculator.xlsx
+++ b/AED withdrawal relapse risk calculator.xlsx
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="58">
-  <si>
-    <t>Nomogram Points</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="58">
   <si>
     <t>ttsf</t>
   </si>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>≥24</t>
-  </si>
-  <si>
-    <t>Total score</t>
   </si>
   <si>
     <t>Risk.2y</t>
@@ -316,11 +310,14 @@
     <t>(select one)</t>
   </si>
   <si>
-    <t>Date of version calculation sheet: 2017-03-16</t>
+    <t>NomogramPoints</t>
+  </si>
+  <si>
+    <t>TotalScore</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Calculation of individual seizure outcome of AED withdrawal for seizure free people with epilepsy. Calculations are based on nomograms as presented in Lamberink et al., </t>
+      <t xml:space="preserve">Calculation of individual seizure outcome of AED withdrawal for seizure free people with epilepsy. Calculations are based on nomograms as presented in </t>
     </r>
     <r>
       <rPr>
@@ -332,7 +329,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Journal</t>
+      <t>The Lancet Neurology 2017</t>
     </r>
     <r>
       <rPr>
@@ -343,7 +340,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, vol(issue):pp-pp.
+      <t xml:space="preserve">, published online May 5, DOI http://dx.doi.org/10.1016/S1474-4422(17)30114-X 
 </t>
     </r>
     <r>
@@ -359,7 +356,10 @@
     </r>
   </si>
   <si>
-    <t>Reference: Journal. 2017. Vol(issue):pp-pp</t>
+    <t xml:space="preserve">Reference: The Lancet Neurology 2017, published online May 5, DOI http://dx.doi.org/10.1016/S1474-4422(17)30114-X </t>
+  </si>
+  <si>
+    <t>Date of version calculation sheet: 2017-05-10</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -555,21 +555,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -579,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -597,10 +582,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -986,7 +967,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,279 +981,279 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
+      <c r="A1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B3,Recur.nomogram!B2:B108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B3,Long.nomogram!B2:B69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>50</v>
+      <c r="A4" s="33" t="s">
+        <v>48</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="21">
+        <v>52</v>
+      </c>
+      <c r="C4" s="20">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B4,Recur.nomogram!C2:C108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B4,Long.nomogram!C2:C69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>35</v>
+      <c r="A5" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21">
+        <v>52</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B5,Long.nomogram!D2:D69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>36</v>
+      <c r="A6" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21">
+        <v>52</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B6,Long.nomogram!E2:E69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>53</v>
+      <c r="A7" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="21">
+        <v>52</v>
+      </c>
+      <c r="C7" s="20">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B7,Recur.nomogram!D2:D108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>44</v>
+      <c r="A8" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21">
+        <v>52</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B8,Long.nomogram!F2:F69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>18</v>
+      <c r="A9" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="21">
+        <v>52</v>
+      </c>
+      <c r="C9" s="20">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B9,Recur.nomogram!E2:E108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>46</v>
+      <c r="A10" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="21">
+        <v>52</v>
+      </c>
+      <c r="C10" s="20">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B10,Recur.nomogram!F2:F108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="20">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B10,Long.nomogram!G2:G69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>45</v>
+      <c r="A11" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="21">
+        <v>52</v>
+      </c>
+      <c r="C11" s="20">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B11,Recur.nomogram!G2:G108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>37</v>
+      <c r="A12" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21">
+        <v>52</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B12,Long.nomogram!H2:H69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>19</v>
+      <c r="A13" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="21">
+        <v>52</v>
+      </c>
+      <c r="C13" s="20">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B13,Recur.nomogram!H2:H108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="21"/>
+      <c r="D13" s="20"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="22">
+      <c r="A14" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="21">
         <f>INDEX(Recur.nomogram!A2:I108,MATCH(B14,Recur.nomogram!I2:I108,0),1)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <f>INDEX(Long.nomogram!A2:I69,MATCH(B14,Long.nomogram!I2:I69,0),1)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="15">
+      <c r="A15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="14">
         <f>SUM(C3:C14)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="14">
         <f>SUM(D3:D14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="23" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="15" t="str">
+        <f>INDEX(Recur.risk!A2:C121,MATCH(C15,Recur.risk!A2:A121,0),2)</f>
+        <v>&lt;10%</v>
+      </c>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="16" t="str">
-        <f>INDEX(Recur.risk!A2:C114,MATCH(C15,Recur.risk!A2:A114,0),2)</f>
+      <c r="C18" s="17" t="str">
+        <f>INDEX(Recur.risk!A2:C121,MATCH(C15,Recur.risk!A2:A121,0),3)</f>
         <v>&lt;10%</v>
       </c>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="18" t="str">
-        <f>INDEX(Recur.risk!A2:C114,MATCH(C15,Recur.risk!A2:A114,0),3)</f>
-        <v>&lt;10%</v>
-      </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="33" t="str">
+      <c r="A19" s="12"/>
+      <c r="B19" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="32" t="str">
         <f>INDEX(Long.risk!A2:B97,MATCH(D15,Long.risk!A2:A97,0),2)</f>
         <v>&gt;99%</v>
       </c>
-      <c r="E19" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-    </row>
-    <row r="20" spans="1:7" s="29" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
+      <c r="E19" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+    </row>
+    <row r="20" spans="1:7" s="28" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="A22" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8D79" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="995D" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E19:E20"/>
@@ -1326,11 +1307,11 @@
   <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2:I107"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:I107"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:I107"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:I2"/>
+      <selection pane="bottomRight" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1342,60 +1323,60 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
+    </row>
+    <row r="2" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
         <v>0</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>54</v>
+      <c r="B2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1406,25 +1387,25 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1476,7 +1457,7 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1495,7 +1476,7 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1509,7 +1490,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1520,7 +1501,7 @@
         <v>20</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1553,7 +1534,7 @@
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1576,7 +1557,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
+      <c r="A18" s="26">
         <v>6.5</v>
       </c>
       <c r="D18">
@@ -1584,7 +1565,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
+      <c r="A19" s="26">
         <v>6.5</v>
       </c>
       <c r="D19">
@@ -1592,7 +1573,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
+      <c r="A20" s="26">
         <v>6.5</v>
       </c>
       <c r="D20">
@@ -1600,7 +1581,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+      <c r="A21" s="26">
         <v>6.5</v>
       </c>
       <c r="D21">
@@ -1608,7 +1589,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="A22" s="26">
         <v>6.5</v>
       </c>
       <c r="D22">
@@ -1616,7 +1597,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
+      <c r="A23" s="26">
         <v>6.5</v>
       </c>
       <c r="D23">
@@ -1624,7 +1605,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
+      <c r="A24" s="26">
         <v>6.5</v>
       </c>
       <c r="D24">
@@ -1632,7 +1613,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="27">
+      <c r="A25" s="26">
         <v>6.5</v>
       </c>
       <c r="D25">
@@ -1640,7 +1621,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
+      <c r="A26" s="26">
         <v>6.5</v>
       </c>
       <c r="D26">
@@ -1648,7 +1629,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="27">
+      <c r="A27" s="26">
         <v>6.5</v>
       </c>
       <c r="D27">
@@ -1656,7 +1637,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="27">
+      <c r="A28" s="26">
         <v>6.5</v>
       </c>
       <c r="D28">
@@ -1664,7 +1645,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
+      <c r="A29" s="26">
         <v>6.5</v>
       </c>
       <c r="D29">
@@ -1672,7 +1653,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="27">
+      <c r="A30" s="26">
         <v>6.5</v>
       </c>
       <c r="D30">
@@ -1680,7 +1661,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="27">
+      <c r="A31" s="26">
         <v>6.5</v>
       </c>
       <c r="D31">
@@ -1688,7 +1669,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="27">
+      <c r="A32" s="26">
         <v>6.5</v>
       </c>
       <c r="D32">
@@ -1696,7 +1677,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="27">
+      <c r="A33" s="26">
         <v>6.5</v>
       </c>
       <c r="D33">
@@ -1704,7 +1685,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="27">
+      <c r="A34" s="26">
         <v>6.5</v>
       </c>
       <c r="D34">
@@ -1712,7 +1693,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="27">
+      <c r="A35" s="26">
         <v>6.5</v>
       </c>
       <c r="D35">
@@ -1720,7 +1701,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
+      <c r="A36" s="26">
         <v>6.5</v>
       </c>
       <c r="D36">
@@ -1728,7 +1709,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
+      <c r="A37" s="26">
         <v>6.5</v>
       </c>
       <c r="D37">
@@ -1736,7 +1717,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
+      <c r="A38" s="26">
         <v>6.5</v>
       </c>
       <c r="D38">
@@ -1744,7 +1725,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="27">
+      <c r="A39" s="26">
         <v>6.5</v>
       </c>
       <c r="D39">
@@ -2210,7 +2191,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="27">
+      <c r="A86" s="26">
         <v>10.5</v>
       </c>
       <c r="B86">
@@ -2221,7 +2202,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="27">
+      <c r="A87" s="26">
         <v>10.5</v>
       </c>
       <c r="B87">
@@ -2232,7 +2213,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="27">
+      <c r="A88" s="26">
         <v>10.5</v>
       </c>
       <c r="D88">
@@ -2240,7 +2221,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="27">
+      <c r="A89" s="26">
         <v>10.5</v>
       </c>
       <c r="D89">
@@ -2248,7 +2229,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="27">
+      <c r="A90" s="26">
         <v>10.5</v>
       </c>
       <c r="D90">
@@ -2256,7 +2237,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="27">
+      <c r="A91" s="26">
         <v>11</v>
       </c>
       <c r="D91">
@@ -2264,7 +2245,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="27">
+      <c r="A92" s="26">
         <v>11</v>
       </c>
       <c r="D92">
@@ -2272,7 +2253,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="27">
+      <c r="A93" s="26">
         <v>11</v>
       </c>
       <c r="D93">
@@ -2280,7 +2261,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="27">
+      <c r="A94" s="26">
         <v>11</v>
       </c>
       <c r="D94">
@@ -2288,7 +2269,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="27">
+      <c r="A95" s="26">
         <v>11</v>
       </c>
       <c r="D95">
@@ -2369,7 +2350,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>20</v>
+        <v>19.5</v>
       </c>
       <c r="C105">
         <v>3</v>
@@ -2400,7 +2381,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8D79" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="995D" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2411,7 +2392,7 @@
   <sheetPr codeName="Blad3"/>
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -2419,54 +2400,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>54</v>
+      <c r="A2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2480,19 +2461,19 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2506,19 +2487,19 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2768,7 +2749,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>24</v>
@@ -3103,7 +3084,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8D79" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="995D" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3112,10 +3093,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad4"/>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C114"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,13 +3106,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3139,1246 +3120,1323 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4.5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5.5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6.5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7.5</v>
-      </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8.5</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>9.5</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>10</v>
+        <v>6.5</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>10.5</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
+        <v>7.5</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>11.5</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>12</v>
+        <v>8.5</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>12.5</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>13</v>
+        <v>9.5</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0.1</v>
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>13.5</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="5">
-        <v>0.10666666666666667</v>
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>14</v>
+        <v>10.5</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0.11333333333333334</v>
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>14.5</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5">
-        <v>0.12000000000000002</v>
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>15</v>
+        <v>11.5</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="5">
-        <v>0.12666666666666668</v>
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>15.5</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0.13333333333333336</v>
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>16</v>
-      </c>
-      <c r="B27" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0.14000000000000001</v>
+        <v>12.5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>16.5</v>
-      </c>
-      <c r="B28" s="5">
-        <v>0.10625000000000001</v>
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
       </c>
       <c r="C28" s="5">
-        <v>0.1466666666666667</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>17</v>
-      </c>
-      <c r="B29" s="5">
-        <v>0.1125</v>
+        <v>13.5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
       </c>
       <c r="C29" s="5">
-        <v>0.15333333333333338</v>
+        <v>0.10666666666666667</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>17.5</v>
-      </c>
-      <c r="B30" s="5">
-        <v>0.11875000000000001</v>
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
       </c>
       <c r="C30" s="5">
-        <v>0.16000000000000003</v>
+        <v>0.11333333333333334</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>18</v>
-      </c>
-      <c r="B31" s="5">
-        <v>0.125</v>
+        <v>14.5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
       </c>
       <c r="C31" s="5">
-        <v>0.16666666666666669</v>
+        <v>0.12000000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>18.5</v>
-      </c>
-      <c r="B32" s="5">
-        <v>0.13125000000000001</v>
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
       </c>
       <c r="C32" s="5">
-        <v>0.17333333333333337</v>
+        <v>0.12666666666666668</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>19</v>
-      </c>
-      <c r="B33" s="5">
-        <v>0.13750000000000001</v>
+        <v>15.5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
       </c>
       <c r="C33" s="5">
-        <v>0.18000000000000005</v>
+        <v>0.13333333333333336</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>19.5</v>
+        <v>16</v>
       </c>
       <c r="B34" s="5">
-        <v>0.14375000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="C34" s="5">
-        <v>0.1866666666666667</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>20</v>
+        <v>16.5</v>
       </c>
       <c r="B35" s="5">
-        <v>0.15000000000000002</v>
+        <v>0.10625000000000001</v>
       </c>
       <c r="C35" s="5">
-        <v>0.19333333333333338</v>
+        <v>0.1466666666666667</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>20.5</v>
+        <v>17</v>
       </c>
       <c r="B36" s="5">
-        <v>0.15625</v>
+        <v>0.1125</v>
       </c>
       <c r="C36" s="5">
-        <v>0.20000000000000007</v>
+        <v>0.15333333333333338</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>21</v>
+        <v>17.5</v>
       </c>
       <c r="B37" s="5">
-        <v>0.16250000000000001</v>
+        <v>0.11875000000000001</v>
       </c>
       <c r="C37" s="5">
-        <v>0.21111111111111117</v>
+        <v>0.16000000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>21.5</v>
+        <v>18</v>
       </c>
       <c r="B38" s="5">
-        <v>0.16875000000000001</v>
+        <v>0.125</v>
       </c>
       <c r="C38" s="5">
-        <v>0.22222222222222227</v>
+        <v>0.16666666666666669</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>22</v>
+        <v>18.5</v>
       </c>
       <c r="B39" s="5">
-        <v>0.17500000000000002</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="C39" s="5">
-        <v>0.23333333333333336</v>
+        <v>0.17333333333333337</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>22.5</v>
+        <v>19</v>
       </c>
       <c r="B40" s="5">
-        <v>0.18125000000000002</v>
+        <v>0.13750000000000001</v>
       </c>
       <c r="C40" s="5">
-        <v>0.24444444444444446</v>
+        <v>0.18000000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>23</v>
+        <v>19.5</v>
       </c>
       <c r="B41" s="5">
-        <v>0.1875</v>
+        <v>0.14375000000000002</v>
       </c>
       <c r="C41" s="5">
-        <v>0.25555555555555554</v>
+        <v>0.1866666666666667</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>23.5</v>
+        <v>20</v>
       </c>
       <c r="B42" s="5">
-        <v>0.19375000000000001</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="C42" s="5">
-        <v>0.26666666666666666</v>
+        <v>0.19333333333333338</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>24</v>
+        <v>20.5</v>
       </c>
       <c r="B43" s="5">
-        <v>0.2</v>
+        <v>0.15625</v>
       </c>
       <c r="C43" s="5">
-        <v>0.27777777777777779</v>
+        <v>0.20000000000000007</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>24.5</v>
+        <v>21</v>
       </c>
       <c r="B44" s="5">
-        <v>0.21111111111111111</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="C44" s="5">
-        <v>0.28888888888888886</v>
+        <v>0.21111111111111117</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>25</v>
+        <v>21.5</v>
       </c>
       <c r="B45" s="5">
-        <v>0.22222222222222221</v>
+        <v>0.16875000000000001</v>
       </c>
       <c r="C45" s="5">
-        <v>0.29999999999999993</v>
+        <v>0.22222222222222227</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>25.5</v>
+        <v>22</v>
       </c>
       <c r="B46" s="5">
-        <v>0.23333333333333331</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="C46" s="5">
-        <v>0.31249999999999994</v>
+        <v>0.23333333333333336</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>26</v>
+        <v>22.5</v>
       </c>
       <c r="B47" s="5">
-        <v>0.24444444444444441</v>
+        <v>0.18125000000000002</v>
       </c>
       <c r="C47" s="5">
-        <v>0.32499999999999996</v>
+        <v>0.24444444444444446</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>26.5</v>
+        <v>23</v>
       </c>
       <c r="B48" s="5">
+        <v>0.1875</v>
+      </c>
+      <c r="C48" s="5">
         <v>0.25555555555555554</v>
-      </c>
-      <c r="C48" s="5">
-        <v>0.33749999999999991</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>27</v>
+        <v>23.5</v>
       </c>
       <c r="B49" s="5">
-        <v>0.26666666666666661</v>
+        <v>0.19375000000000001</v>
       </c>
       <c r="C49" s="5">
-        <v>0.34999999999999992</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>27.5</v>
+        <v>24</v>
       </c>
       <c r="B50" s="5">
-        <v>0.27777777777777768</v>
+        <v>0.2</v>
       </c>
       <c r="C50" s="5">
-        <v>0.36249999999999993</v>
+        <v>0.27777777777777779</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>28</v>
+        <v>24.5</v>
       </c>
       <c r="B51" s="5">
-        <v>0.28888888888888881</v>
+        <v>0.21111111111111111</v>
       </c>
       <c r="C51" s="5">
-        <v>0.37499999999999994</v>
+        <v>0.28888888888888886</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>28.5</v>
+        <v>25</v>
       </c>
       <c r="B52" s="5">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="C52" s="5">
         <v>0.29999999999999993</v>
-      </c>
-      <c r="C52" s="5">
-        <v>0.38749999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>29</v>
+        <v>25.5</v>
       </c>
       <c r="B53" s="5">
-        <v>0.31428571428571422</v>
+        <v>0.23333333333333331</v>
       </c>
       <c r="C53" s="5">
-        <v>0.39999999999999991</v>
+        <v>0.31249999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>29.5</v>
+        <v>26</v>
       </c>
       <c r="B54" s="5">
-        <v>0.32857142857142851</v>
+        <v>0.24444444444444441</v>
       </c>
       <c r="C54" s="5">
-        <v>0.41666666666666663</v>
+        <v>0.32499999999999996</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>30</v>
+        <v>26.5</v>
       </c>
       <c r="B55" s="5">
-        <v>0.34285714285714286</v>
+        <v>0.25555555555555554</v>
       </c>
       <c r="C55" s="5">
-        <v>0.43333333333333329</v>
+        <v>0.33749999999999991</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>30.5</v>
+        <v>27</v>
       </c>
       <c r="B56" s="5">
-        <v>0.35714285714285715</v>
+        <v>0.26666666666666661</v>
       </c>
       <c r="C56" s="5">
-        <v>0.45</v>
+        <v>0.34999999999999992</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>31</v>
+        <v>27.5</v>
       </c>
       <c r="B57" s="5">
-        <v>0.37142857142857144</v>
+        <v>0.27777777777777768</v>
       </c>
       <c r="C57" s="5">
-        <v>0.46666666666666673</v>
+        <v>0.36249999999999993</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>31.5</v>
+        <v>28</v>
       </c>
       <c r="B58" s="5">
-        <v>0.38571428571428573</v>
+        <v>0.28888888888888881</v>
       </c>
       <c r="C58" s="5">
-        <v>0.48333333333333339</v>
+        <v>0.37499999999999994</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>32</v>
+        <v>28.5</v>
       </c>
       <c r="B59" s="5">
-        <v>0.4</v>
+        <v>0.29999999999999993</v>
       </c>
       <c r="C59" s="5">
-        <v>0.50000000000000011</v>
+        <v>0.38749999999999996</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>32.5</v>
+        <v>29</v>
       </c>
       <c r="B60" s="5">
-        <v>0.41428571428571431</v>
+        <v>0.31428571428571422</v>
       </c>
       <c r="C60" s="5">
-        <v>0.51666666666666672</v>
+        <v>0.39999999999999991</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>33</v>
+        <v>29.5</v>
       </c>
       <c r="B61" s="5">
-        <v>0.4285714285714286</v>
+        <v>0.32857142857142851</v>
       </c>
       <c r="C61" s="5">
-        <v>0.53333333333333333</v>
+        <v>0.41666666666666663</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>33.5</v>
+        <v>30</v>
       </c>
       <c r="B62" s="5">
-        <v>0.44285714285714295</v>
+        <v>0.34285714285714286</v>
       </c>
       <c r="C62" s="5">
-        <v>0.54999999999999993</v>
+        <v>0.43333333333333329</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>34</v>
+        <v>30.5</v>
       </c>
       <c r="B63" s="5">
-        <v>0.45714285714285724</v>
+        <v>0.35714285714285715</v>
       </c>
       <c r="C63" s="5">
-        <v>0.56666666666666654</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>34.5</v>
+        <v>31</v>
       </c>
       <c r="B64" s="5">
-        <v>0.47142857142857153</v>
+        <v>0.37142857142857144</v>
       </c>
       <c r="C64" s="5">
-        <v>0.58333333333333315</v>
+        <v>0.46666666666666673</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>35</v>
+        <v>31.5</v>
       </c>
       <c r="B65" s="5">
-        <v>0.48571428571428582</v>
+        <v>0.38571428571428573</v>
       </c>
       <c r="C65" s="5">
-        <v>0.59999999999999976</v>
+        <v>0.48333333333333339</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="B66" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C66" s="5">
         <v>0.50000000000000011</v>
-      </c>
-      <c r="C66" s="5">
-        <v>0.61999999999999977</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>36</v>
+        <v>32.5</v>
       </c>
       <c r="B67" s="5">
+        <v>0.41428571428571431</v>
+      </c>
+      <c r="C67" s="5">
         <v>0.51666666666666672</v>
-      </c>
-      <c r="C67" s="5">
-        <v>0.63999999999999979</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>36.5</v>
+        <v>33</v>
       </c>
       <c r="B68" s="5">
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="C68" s="5">
         <v>0.53333333333333333</v>
-      </c>
-      <c r="C68" s="5">
-        <v>0.6599999999999997</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>37</v>
+        <v>33.5</v>
       </c>
       <c r="B69" s="5">
+        <v>0.44285714285714295</v>
+      </c>
+      <c r="C69" s="5">
         <v>0.54999999999999993</v>
-      </c>
-      <c r="C69" s="5">
-        <v>0.67999999999999972</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>37.5</v>
+        <v>34</v>
       </c>
       <c r="B70" s="5">
+        <v>0.45714285714285724</v>
+      </c>
+      <c r="C70" s="5">
         <v>0.56666666666666654</v>
-      </c>
-      <c r="C70" s="5">
-        <v>0.69999999999999973</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>38</v>
+        <v>34.5</v>
       </c>
       <c r="B71" s="5">
+        <v>0.47142857142857153</v>
+      </c>
+      <c r="C71" s="5">
         <v>0.58333333333333315</v>
-      </c>
-      <c r="C71" s="5">
-        <v>0.71666666666666645</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>38.5</v>
+        <v>35</v>
       </c>
       <c r="B72" s="5">
+        <v>0.48571428571428582</v>
+      </c>
+      <c r="C72" s="5">
         <v>0.59999999999999976</v>
-      </c>
-      <c r="C72" s="5">
-        <v>0.73333333333333317</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>39</v>
+        <v>35.5</v>
       </c>
       <c r="B73" s="5">
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="C73" s="5">
         <v>0.61999999999999977</v>
-      </c>
-      <c r="C73" s="5">
-        <v>0.74999999999999978</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>39.5</v>
+        <v>36</v>
       </c>
       <c r="B74" s="5">
+        <v>0.51666666666666672</v>
+      </c>
+      <c r="C74" s="5">
         <v>0.63999999999999979</v>
-      </c>
-      <c r="C74" s="5">
-        <v>0.7666666666666665</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>40</v>
+        <v>36.5</v>
       </c>
       <c r="B75" s="5">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="C75" s="5">
         <v>0.6599999999999997</v>
-      </c>
-      <c r="C75" s="5">
-        <v>0.78333333333333321</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>40.5</v>
+        <v>37</v>
       </c>
       <c r="B76" s="5">
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="C76" s="5">
         <v>0.67999999999999972</v>
-      </c>
-      <c r="C76" s="5">
-        <v>0.79999999999999993</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>41</v>
+        <v>37.5</v>
       </c>
       <c r="B77" s="5">
+        <v>0.56666666666666654</v>
+      </c>
+      <c r="C77" s="5">
         <v>0.69999999999999973</v>
-      </c>
-      <c r="C77" s="5">
-        <v>0.81428571428571428</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>41.5</v>
+        <v>38</v>
       </c>
       <c r="B78" s="5">
+        <v>0.58333333333333315</v>
+      </c>
+      <c r="C78" s="5">
         <v>0.71666666666666645</v>
-      </c>
-      <c r="C78" s="5">
-        <v>0.82857142857142851</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>42</v>
+        <v>38.5</v>
       </c>
       <c r="B79" s="5">
+        <v>0.59999999999999976</v>
+      </c>
+      <c r="C79" s="5">
         <v>0.73333333333333317</v>
-      </c>
-      <c r="C79" s="5">
-        <v>0.84285714285714286</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>42.5</v>
+        <v>39</v>
       </c>
       <c r="B80" s="5">
+        <v>0.61999999999999977</v>
+      </c>
+      <c r="C80" s="5">
         <v>0.74999999999999978</v>
-      </c>
-      <c r="C80" s="5">
-        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>43</v>
+        <v>39.5</v>
       </c>
       <c r="B81" s="5">
+        <v>0.63999999999999979</v>
+      </c>
+      <c r="C81" s="5">
         <v>0.7666666666666665</v>
-      </c>
-      <c r="C81" s="5">
-        <v>0.87142857142857144</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>43.5</v>
+        <v>40</v>
       </c>
       <c r="B82" s="5">
+        <v>0.6599999999999997</v>
+      </c>
+      <c r="C82" s="5">
         <v>0.78333333333333321</v>
-      </c>
-      <c r="C82" s="5">
-        <v>0.88571428571428568</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>44</v>
+        <v>40.5</v>
       </c>
       <c r="B83" s="5">
+        <v>0.67999999999999972</v>
+      </c>
+      <c r="C83" s="5">
         <v>0.79999999999999993</v>
-      </c>
-      <c r="C83" s="5">
-        <v>0.9</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>44.5</v>
+        <v>41</v>
       </c>
       <c r="B84" s="5">
+        <v>0.69999999999999973</v>
+      </c>
+      <c r="C84" s="5">
         <v>0.81428571428571428</v>
-      </c>
-      <c r="C84" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>45</v>
+        <v>41.5</v>
       </c>
       <c r="B85" s="5">
+        <v>0.71666666666666645</v>
+      </c>
+      <c r="C85" s="5">
         <v>0.82857142857142851</v>
-      </c>
-      <c r="C85" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>45.5</v>
+        <v>42</v>
       </c>
       <c r="B86" s="5">
+        <v>0.73333333333333317</v>
+      </c>
+      <c r="C86" s="5">
         <v>0.84285714285714286</v>
-      </c>
-      <c r="C86" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>46</v>
+        <v>42.5</v>
       </c>
       <c r="B87" s="5">
+        <v>0.74999999999999978</v>
+      </c>
+      <c r="C87" s="5">
         <v>0.8571428571428571</v>
-      </c>
-      <c r="C87" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>46.5</v>
+        <v>43</v>
       </c>
       <c r="B88" s="5">
+        <v>0.7666666666666665</v>
+      </c>
+      <c r="C88" s="5">
         <v>0.87142857142857144</v>
-      </c>
-      <c r="C88" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>47</v>
+        <v>43.5</v>
       </c>
       <c r="B89" s="5">
+        <v>0.78333333333333321</v>
+      </c>
+      <c r="C89" s="5">
         <v>0.88571428571428568</v>
-      </c>
-      <c r="C89" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>47.5</v>
+        <v>44</v>
       </c>
       <c r="B90" s="5">
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="C90" s="5">
         <v>0.9</v>
-      </c>
-      <c r="C90" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>48</v>
-      </c>
-      <c r="B91" t="s">
-        <v>27</v>
+        <v>44.5</v>
+      </c>
+      <c r="B91" s="5">
+        <v>0.81428571428571428</v>
       </c>
       <c r="C91" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>48.5</v>
-      </c>
-      <c r="B92" t="s">
-        <v>27</v>
+        <v>45</v>
+      </c>
+      <c r="B92" s="5">
+        <v>0.82857142857142851</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>49</v>
-      </c>
-      <c r="B93" t="s">
-        <v>27</v>
+        <v>45.5</v>
+      </c>
+      <c r="B93" s="5">
+        <v>0.84285714285714286</v>
       </c>
       <c r="C93" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>49.5</v>
-      </c>
-      <c r="B94" t="s">
-        <v>27</v>
+        <v>46</v>
+      </c>
+      <c r="B94" s="5">
+        <v>0.8571428571428571</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>50</v>
-      </c>
-      <c r="B95" t="s">
-        <v>27</v>
+        <v>46.5</v>
+      </c>
+      <c r="B95" s="5">
+        <v>0.87142857142857144</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>50.5</v>
-      </c>
-      <c r="B96" t="s">
-        <v>27</v>
+        <v>47</v>
+      </c>
+      <c r="B96" s="5">
+        <v>0.88571428571428568</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>51</v>
-      </c>
-      <c r="B97" t="s">
-        <v>27</v>
+        <v>47.5</v>
+      </c>
+      <c r="B97" s="5">
+        <v>0.9</v>
       </c>
       <c r="C97" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>51.5</v>
+        <v>48</v>
       </c>
       <c r="B98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C98" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>52</v>
+        <v>48.5</v>
       </c>
       <c r="B99" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C99" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>52.5</v>
+        <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>53</v>
+        <v>49.5</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C101" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>53.5</v>
+        <v>50</v>
       </c>
       <c r="B102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C102" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>54</v>
+        <v>50.5</v>
       </c>
       <c r="B103" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C103" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>54.5</v>
+        <v>51</v>
       </c>
       <c r="B104" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C104" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>55</v>
+        <v>51.5</v>
       </c>
       <c r="B105" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C105" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>55.5</v>
+        <v>52</v>
       </c>
       <c r="B106" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>56</v>
+        <v>52.5</v>
       </c>
       <c r="B107" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C107" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>56.5</v>
+        <v>53</v>
       </c>
       <c r="B108" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C108" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>57</v>
+        <v>53.5</v>
       </c>
       <c r="B109" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C109" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>57.5</v>
+        <v>54</v>
       </c>
       <c r="B110" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C110" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>58</v>
+        <v>54.5</v>
       </c>
       <c r="B111" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C111" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>58.5</v>
+        <v>55</v>
       </c>
       <c r="B112" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C112" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>59</v>
+        <v>55.5</v>
       </c>
       <c r="B113" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C113" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
+        <v>56</v>
+      </c>
+      <c r="B114" t="s">
+        <v>25</v>
+      </c>
+      <c r="C114" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>56.5</v>
+      </c>
+      <c r="B115" t="s">
+        <v>25</v>
+      </c>
+      <c r="C115" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>57</v>
+      </c>
+      <c r="B116" t="s">
+        <v>25</v>
+      </c>
+      <c r="C116" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>57.5</v>
+      </c>
+      <c r="B117" t="s">
+        <v>25</v>
+      </c>
+      <c r="C117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>58</v>
+      </c>
+      <c r="B118" t="s">
+        <v>25</v>
+      </c>
+      <c r="C118" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>58.5</v>
+      </c>
+      <c r="B119" t="s">
+        <v>25</v>
+      </c>
+      <c r="C119" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>59</v>
+      </c>
+      <c r="B120" t="s">
+        <v>25</v>
+      </c>
+      <c r="C120" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
         <v>59.5</v>
       </c>
-      <c r="B114" t="s">
-        <v>27</v>
-      </c>
-      <c r="C114" t="s">
-        <v>27</v>
+      <c r="B121" t="s">
+        <v>25</v>
+      </c>
+      <c r="C121" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8D79" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="995D" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4393,7 +4451,7 @@
       <selection activeCell="A2" sqref="A2:I107"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:I107"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:I107"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:I2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4404,60 +4462,60 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
         <v>0</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>54</v>
+      <c r="B2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -4468,25 +4526,25 @@
         <v>0</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -4511,7 +4569,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -4522,10 +4580,10 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -4536,7 +4594,7 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -4553,7 +4611,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -5051,7 +5109,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8D79" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="995D" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5075,54 +5133,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>54</v>
+      <c r="A2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5136,19 +5194,19 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5162,19 +5220,19 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5223,7 +5281,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -5328,11 +5386,11 @@
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8D79" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="995D" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5351,10 +5409,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -5362,7 +5420,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5370,7 +5428,7 @@
         <v>0.5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5378,7 +5436,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5386,7 +5444,7 @@
         <v>1.5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5394,7 +5452,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5402,7 +5460,7 @@
         <v>2.5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5410,7 +5468,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -5418,7 +5476,7 @@
         <v>3.5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5426,7 +5484,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5434,7 +5492,7 @@
         <v>4.5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5442,7 +5500,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5450,7 +5508,7 @@
         <v>5.5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -5458,7 +5516,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -5466,7 +5524,7 @@
         <v>6.5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5474,7 +5532,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -5482,7 +5540,7 @@
         <v>7.5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -5490,7 +5548,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5498,7 +5556,7 @@
         <v>8.5</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -5506,7 +5564,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5514,7 +5572,7 @@
         <v>9.5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -5522,7 +5580,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -5530,7 +5588,7 @@
         <v>10.5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5538,7 +5596,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5546,7 +5604,7 @@
         <v>11.5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -5554,7 +5612,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -5562,7 +5620,7 @@
         <v>12.5</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5570,7 +5628,7 @@
         <v>13</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -5578,7 +5636,7 @@
         <v>13.5</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -5586,7 +5644,7 @@
         <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -5594,7 +5652,7 @@
         <v>14.5</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -5938,7 +5996,7 @@
         <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -5946,7 +6004,7 @@
         <v>36.5</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -5954,7 +6012,7 @@
         <v>37</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -5962,7 +6020,7 @@
         <v>37.5</v>
       </c>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -5970,7 +6028,7 @@
         <v>38</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -5978,7 +6036,7 @@
         <v>38.5</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -5986,7 +6044,7 @@
         <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -5994,7 +6052,7 @@
         <v>39.5</v>
       </c>
       <c r="B81" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -6002,7 +6060,7 @@
         <v>40</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -6010,7 +6068,7 @@
         <v>40.5</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -6018,7 +6076,7 @@
         <v>41</v>
       </c>
       <c r="B84" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -6026,7 +6084,7 @@
         <v>41.5</v>
       </c>
       <c r="B85" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -6034,7 +6092,7 @@
         <v>42</v>
       </c>
       <c r="B86" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -6042,7 +6100,7 @@
         <v>42.5</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -6050,7 +6108,7 @@
         <v>43</v>
       </c>
       <c r="B88" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -6058,7 +6116,7 @@
         <v>43.5</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -6066,7 +6124,7 @@
         <v>44</v>
       </c>
       <c r="B90" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -6074,7 +6132,7 @@
         <v>44.5</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -6082,7 +6140,7 @@
         <v>45</v>
       </c>
       <c r="B92" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -6090,7 +6148,7 @@
         <v>45.5</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -6098,7 +6156,7 @@
         <v>46</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -6106,7 +6164,7 @@
         <v>46.5</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -6114,7 +6172,7 @@
         <v>47</v>
       </c>
       <c r="B96" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -6122,11 +6180,11 @@
         <v>47.5</v>
       </c>
       <c r="B97" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="8D79" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="995D" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>